<commit_message>
First Commint for Amazon
</commit_message>
<xml_diff>
--- a/AdactinHotelBooking/src/test/resources/DataProvider/DataSearchHotel.xlsx
+++ b/AdactinHotelBooking/src/test/resources/DataProvider/DataSearchHotel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-workspace\AdactinHotelBooking\src\test\resources\DataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkingDirectory\AdactinHotelBooking\src\test\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E950EB32-DF12-47F4-B52B-9A795E96D660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BDC59-59A8-481B-AA8E-DED1D175FE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3396" yWindow="2316" windowWidth="17280" windowHeight="8964" xr2:uid="{7CF96BFE-1DC5-4F30-AC73-81B4FCA6E0EC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{7CF96BFE-1DC5-4F30-AC73-81B4FCA6E0EC}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchHotel" sheetId="1" r:id="rId1"/>
@@ -122,10 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,23 +441,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708F3FFA-B34F-4AAA-8785-99ACE33278CC}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -507,6 +508,12 @@
       <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>